<commit_message>
Test Cases updated with: 1) Basic App testcases 2) Smartphone overuse testcases 3) Login test results
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -5,18 +5,19 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\testing\bootstrap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Bootstrap" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
-    <sheet name="BasicApp" sheetId="3" r:id="rId3"/>
-    <sheet name="DeleteLocation" sheetId="4" r:id="rId4"/>
-    <sheet name="Usage Heatmap" sheetId="5" r:id="rId5"/>
+    <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
+    <sheet name="Bootstrap" sheetId="1" r:id="rId2"/>
+    <sheet name="Login" sheetId="2" r:id="rId3"/>
+    <sheet name="BasicApp" sheetId="3" r:id="rId4"/>
+    <sheet name="DeleteLocation" sheetId="4" r:id="rId5"/>
+    <sheet name="SmartPhoneUsageHeatmap" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="154">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -327,13 +328,205 @@
   </si>
   <si>
     <t>admin will enter mac address, start date and end date. And the records that matches the input will be deleted</t>
+  </si>
+  <si>
+    <t>TEST Plan</t>
+  </si>
+  <si>
+    <t>Who are responsible for it?</t>
+  </si>
+  <si>
+    <t>When to do it? Frequency etc</t>
+  </si>
+  <si>
+    <t>PM of the iteration</t>
+  </si>
+  <si>
+    <t>Every Thursday after functions completed</t>
+  </si>
+  <si>
+    <t>Friday and over the weekends</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Fix the bugs in pairs</t>
+  </si>
+  <si>
+    <t>When to fix bugs?</t>
+  </si>
+  <si>
+    <t>Test Setup (People / Computers etc)</t>
+  </si>
+  <si>
+    <t>PM with own laptop</t>
+  </si>
+  <si>
+    <t>This is home page for student users!</t>
+  </si>
+  <si>
+    <t>invalid username/password</t>
+  </si>
+  <si>
+    <t>Error Message saying field should not be empty</t>
+  </si>
+  <si>
+    <t>error msg:" pls fill out this fied</t>
+  </si>
+  <si>
+    <t>error msg:" pls fill out this fied on username field</t>
+  </si>
+  <si>
+    <t>error msg:" pls fill out this fied on password field</t>
+  </si>
+  <si>
+    <t>A homepage with all the functions an admin can access</t>
+  </si>
+  <si>
+    <t>This is home page for admin!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error msg:" pls fill out this fied </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unable to check as given password is numerical. </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>check for blank fields</t>
+  </si>
+  <si>
+    <t>no input</t>
+  </si>
+  <si>
+    <t>just click submit</t>
+  </si>
+  <si>
+    <t>error msg: please fill in all the fields</t>
+  </si>
+  <si>
+    <t>invalid timestamp</t>
+  </si>
+  <si>
+    <t>invalid timestamp format</t>
+  </si>
+  <si>
+    <t>enter wrong format of timing</t>
+  </si>
+  <si>
+    <t>error msg: please fill in correct timestamp</t>
+  </si>
+  <si>
+    <t>valid start date and end date</t>
+  </si>
+  <si>
+    <t>start time and end time</t>
+  </si>
+  <si>
+    <t>enter a start time and end time</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked year,checked gender and checked school option</t>
+  </si>
+  <si>
+    <t>start date and end date with all three additional check box info checked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter start time and end time and tick all the boxes. </t>
+  </si>
+  <si>
+    <t>3  tables for each usage level with the count of users in the category</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked year option</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked gender option</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked school option</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked year and checked gender option</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked year and checked school option</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked gender and checked school option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time plus checked year option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time plus checked gender option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time plus checked school option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time  plus checked year and checked gender option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time plus checked year and checked school option</t>
+  </si>
+  <si>
+    <t>enter a start time and end time  plus checked gender and checked school option</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised by gender then year and then school</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised by gender then school</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised by  year and then school</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised by gender then year</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised  school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3  tables for each usage level. Users break down and categorised by gender </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3  tables for each usage level. Users break down and categorised by year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid start and end time </t>
+  </si>
+  <si>
+    <t>1 table and categorized by app name and each app shows the daily usage hours and percentage</t>
+  </si>
+  <si>
+    <t>start date and end date</t>
+  </si>
+  <si>
+    <t>valid start and end time</t>
+  </si>
+  <si>
+    <t>start time and end time in the right format</t>
+  </si>
+  <si>
+    <t>enter start and and time and click submit</t>
+  </si>
+  <si>
+    <t>A report with the overusae inex value together with the status set to either OVERUSE,NORMAL,TO_BE_CAUTIOUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -379,16 +572,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -396,8 +644,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -413,8 +676,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -428,23 +692,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -452,8 +704,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="15" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
+    <cellStyle name="Calculation" xfId="15" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -805,10 +1097,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="82.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
+      <c r="A1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -822,13 +1183,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -999,34 +1360,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="6" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="25.58203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="12.08203125" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="6"/>
+    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.58203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1054,302 +1415,392 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="3" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="G4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="G5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="G6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="G14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="15">
+        <v>14</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="C16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="G16" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="15">
+        <v>15</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="G17" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
     </row>
@@ -1362,12 +1813,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1381,16 +1832,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1418,493 +1869,611 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="C3" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="B4" s="19"/>
+      <c r="C4" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="15">
         <v>9</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="17">
         <v>10</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
+      <c r="C12" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="17">
         <v>11</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="17">
         <v>13</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="17">
         <v>14</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="B16" s="19"/>
+      <c r="C16" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="17">
         <v>15</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="17">
         <v>16</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="17">
         <v>17</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="17">
         <v>18</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="A21" s="17">
         <v>19</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
+      <c r="C22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A23" s="15">
         <v>21</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
+      <c r="A24" s="15">
         <v>22</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
+      <c r="A25" s="15">
         <v>23</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
+      <c r="A26" s="15">
         <v>24</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+      <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
+      <c r="A28" s="15">
         <v>26</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
+      <c r="A29" s="15">
         <v>27</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
+      <c r="A30" s="15">
         <v>28</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
+      <c r="A31" s="15">
         <v>29</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
+      <c r="C32" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
+      <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
+      <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
+      <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
+      <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
+      <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
+      <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
+      <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
+      <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
+      <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
+      <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1915,14 +2484,15 @@
     <mergeCell ref="B32:B42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1939,16 +2509,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1977,150 +2547,150 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="93" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
-      <c r="A4" s="11">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="11">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="11">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="11">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="11">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2130,34 +2700,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="6"/>
-    <col min="2" max="2" width="58.1640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="20.25" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.4140625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="6"/>
+    <col min="1" max="1" width="8.6640625" style="5"/>
+    <col min="2" max="2" width="58.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.25" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.4140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -2185,53 +2755,81 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="B3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated bootstrap test case, bs-test-5 and bs-test-6
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="19420" windowHeight="12220" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -106,9 +101,6 @@
     <t>File: bs-test-6.zip</t>
   </si>
   <si>
-    <t>Bootstrap success. However, 7 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9 will not be displayed in the database. All other rows should be displayed correctly.</t>
-  </si>
-  <si>
     <t>Bootstrap success. However, 6 error messages are returned to admin. Row 1,2 will consist of mac-address "invalid mac address" error. Row 3 will consist of mac-address "no matching mac address" error. Row 5 will consist of app-id error. Row 7 will consist of incorrect timestamp error. Row 10 will consist of a duplicated of row 9. Rows 1,2,3,5,7,9 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
   <si>
@@ -520,6 +512,9 @@
   </si>
   <si>
     <t>A report with the overusae inex value together with the status set to either OVERUSE,NORMAL,TO_BE_CAUTIOUS</t>
+  </si>
+  <si>
+    <t>Bootstrap success. However, 7 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
 </sst>
 </file>
@@ -710,18 +705,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -735,13 +718,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1110,49 +1105,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
-      <c r="A1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="11"/>
+      <c r="A1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1168,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1183,13 +1178,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1238,7 +1233,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="124" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1255,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
@@ -1295,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
@@ -1315,7 +1310,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
@@ -1335,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1364,7 +1359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1381,20 +1376,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1420,25 +1415,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1446,25 +1441,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1472,25 +1467,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1498,25 +1493,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1524,22 +1519,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="F7" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
@@ -1547,25 +1542,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
@@ -1573,25 +1568,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1599,25 +1594,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1625,22 +1620,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1648,25 +1643,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1674,25 +1669,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1700,25 +1695,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1726,77 +1721,77 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="5" t="s">
+      <c r="E16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
-        <v>14</v>
-      </c>
-      <c r="B16" s="16" t="s">
+    <row r="17" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C17" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="E17" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
-        <v>15</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>112</v>
+      <c r="F17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1832,13 +1827,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -1870,610 +1865,610 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C12" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E12" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F12" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20" t="s">
+      <c r="D13" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E13" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F13" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="20" t="s">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="13">
+        <v>13</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="13">
+        <v>14</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="13">
+        <v>15</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="13">
+        <v>16</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="13">
+        <v>17</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="13">
+        <v>18</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="13">
+        <v>19</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>20</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>21</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
-        <v>9</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="17">
-        <v>10</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="17">
-        <v>11</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
-        <v>12</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="17">
-        <v>13</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
-        <v>14</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="17">
-        <v>16</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="17">
-        <v>17</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="17">
-        <v>18</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="17">
-        <v>19</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="15">
-        <v>20</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="15">
-        <v>21</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="s">
+      <c r="F23" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="15">
+      <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="15">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="15">
+      <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="15">
+      <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+      <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="15">
+      <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="15">
+      <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="15">
+      <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="E32" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2509,13 +2504,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -2551,19 +2546,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2573,19 +2568,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -2595,13 +2590,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2721,13 +2716,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -2759,18 +2754,18 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
@@ -2778,19 +2773,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update testcases for bootscrap
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="1340" yWindow="60" windowWidth="19420" windowHeight="12160" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="DeleteLocation" sheetId="4" r:id="rId5"/>
     <sheet name="SmartPhoneUsageHeatmap" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -106,16 +101,7 @@
     <t>File: bs-test-6.zip</t>
   </si>
   <si>
-    <t>Bootstrap success. However, 7 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9 will not be displayed in the database. All other rows should be displayed correctly.</t>
-  </si>
-  <si>
     <t>Bootstrap success. However, 6 error messages are returned to admin. Row 1,2 will consist of mac-address "invalid mac address" error. Row 3 will consist of mac-address "no matching mac address" error. Row 5 will consist of app-id error. Row 7 will consist of incorrect timestamp error. Row 10 will consist of a duplicated of row 9. Rows 1,2,3,5,7,9 will not be displayed in the database. All other rows should be displayed correctly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bootstrap success. However, 3 error messages are returned to admin. Row 1,2 will consist of invalid location id error. Row 8,9,10 will consist of invalid semantic place error. Rows 1,2,8,9,10 will not be displayed in the database. All other rows should be displayed correctly. </t>
-  </si>
-  <si>
-    <t>Bootstrap success. However, 4 error messages are returned to admin. Row 1 will consist of invalid location-id error. Row 5,6,20 will consist of invalid mac address error. Row 7 will consist of invalid timestamp error. Row 9 will consist of a duplicate of row 8. Rows 1,5,6,7,9,20 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
   <si>
     <t>Functionality 
@@ -520,6 +506,15 @@
   </si>
   <si>
     <t>A report with the overusae inex value together with the status set to either OVERUSE,NORMAL,TO_BE_CAUTIOUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap success. However, 5 error messages are returned to admin. Row 1,2 will consist of invalid location id error. Row 8,9,10 will consist of invalid semantic place error. Rows 1,2,8,9,10 will not be displayed in the database. All other rows should be displayed correctly. </t>
+  </si>
+  <si>
+    <t>Bootstrap success. However, 6 error messages are returned to admin. Row 1 will consist of invalid location-id error. Row 5,6,20 will consist of invalid mac address error. Row 7 will consist of invalid timestamp error. Row 9 will consist of a duplicate of row 8. Rows 1,5,6,7,9,20 will not be displayed in the database. All other rows should be displayed correctly.</t>
+  </si>
+  <si>
+    <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
 </sst>
 </file>
@@ -710,18 +705,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -735,13 +718,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1110,49 +1105,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
-      <c r="A1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="11"/>
+      <c r="A1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="17"/>
     </row>
     <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1168,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1183,13 +1178,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1238,7 +1233,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="124" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1255,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
@@ -1295,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
@@ -1315,7 +1310,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
@@ -1335,7 +1330,11 @@
         <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>27</v>
+        <v>151</v>
+      </c>
+      <c r="G8">
+        <f>SUM(33-5)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1364,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1381,20 +1380,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1420,25 +1419,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1446,25 +1445,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1472,25 +1471,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1498,25 +1497,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1524,22 +1523,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
@@ -1547,25 +1546,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
@@ -1573,25 +1572,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="H9" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1599,25 +1598,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1625,22 +1624,22 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1648,25 +1647,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1674,25 +1673,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1700,25 +1699,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
@@ -1726,77 +1725,77 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="15">
-        <v>14</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="15">
-        <v>15</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>112</v>
+      <c r="F17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1832,13 +1831,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -1870,610 +1869,610 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="E4" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20" t="s">
+      <c r="F4" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="D5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="E5" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="F5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D14" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E14" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F14" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="13">
+        <v>13</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="13">
+        <v>14</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="13">
+        <v>15</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="15">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="15">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="15">
-        <v>8</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="15">
-        <v>9</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="17">
-        <v>10</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="D17" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="13">
+        <v>16</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="13">
+        <v>17</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="13">
+        <v>18</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="13">
+        <v>19</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>20</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="17">
-        <v>11</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="20" t="s">
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>21</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17">
-        <v>12</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="17">
-        <v>13</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17">
-        <v>14</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="20" t="s">
+      <c r="F23" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="17">
-        <v>16</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="17">
-        <v>17</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="17">
-        <v>18</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="17">
-        <v>19</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="15">
-        <v>20</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="15">
-        <v>21</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="15">
+      <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="15">
+      <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="15">
+      <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="15">
+      <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="15">
+      <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="15">
+      <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="15">
+      <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="15">
+      <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2509,13 +2508,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -2551,19 +2550,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2573,19 +2572,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -2595,13 +2594,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2721,13 +2720,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -2759,18 +2758,18 @@
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
@@ -2778,19 +2777,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added test cases for add batch
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\testing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="60" windowWidth="19420" windowHeight="12160" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
     <sheet name="Bootstrap" sheetId="1" r:id="rId2"/>
-    <sheet name="Login" sheetId="2" r:id="rId3"/>
-    <sheet name="BasicApp" sheetId="3" r:id="rId4"/>
-    <sheet name="DeleteLocation" sheetId="4" r:id="rId5"/>
-    <sheet name="SmartPhoneUsageHeatmap" sheetId="5" r:id="rId6"/>
+    <sheet name="AddBatch" sheetId="7" r:id="rId3"/>
+    <sheet name="Login" sheetId="2" r:id="rId4"/>
+    <sheet name="BasicApp" sheetId="3" r:id="rId5"/>
+    <sheet name="DeleteLocation" sheetId="4" r:id="rId6"/>
+    <sheet name="SmartPhoneUsageHeatmap" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="168">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -51,9 +57,6 @@
   </si>
   <si>
     <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>Boostrap</t>
   </si>
   <si>
     <t>Validate that zip file with the correct file names,file type, number of files, input can be bootstrapped successfully.</t>
@@ -515,13 +518,58 @@
   </si>
   <si>
     <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
+  </si>
+  <si>
+    <t>File: ab-test-1.zip</t>
+  </si>
+  <si>
+    <t>File: ab-test-2.zip</t>
+  </si>
+  <si>
+    <t>Error messages from validation in app.csv (based on app-id,mac-address,timestamp) are returned to admin correctly.</t>
+  </si>
+  <si>
+    <t>File: ab-test-3.zip</t>
+  </si>
+  <si>
+    <t>AddBatch success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddBatch success. However, 18 error messages are returned to admin.  Rows 3, 4, 5 have invalid timestamp, Rows 3, 5, 9, 11, 15 have duplicate mac address, Row 14 has invalid appid, Row 16 has no matching appid, </t>
+  </si>
+  <si>
+    <t>AddBatch</t>
+  </si>
+  <si>
+    <t>BootStrap</t>
+  </si>
+  <si>
+    <t>Addbatch Success. Rows 2, 5, 7, 22, 26 have invalid timestamp. Rows 5, 10, 16, 22, 27, 28 have invalid location. Rows 5, 11, 21, 24 and 25 as well as 29 and 31. Rows 13, 24, 28 and 32 have duplicate mac addresses, but not duplicate timestamp. Rows 3, 4, 8, 12, 17, 19, 20 and 30 are duplicates in the database while rows 6, 9, 13, 14, 15, 18, 23, 25, 32.</t>
+  </si>
+  <si>
+    <t>File ab-test-4.zip</t>
+  </si>
+  <si>
+    <t>File ab-test-5.zip</t>
+  </si>
+  <si>
+    <t>No error messages should be thrown. All files have unique records except for demographics.csv (assumed unique)</t>
+  </si>
+  <si>
+    <t>Addbatch success, no error messages.</t>
+  </si>
+  <si>
+    <t>AddBatch success. However, error messages for app.csv and location.csv should be returned as all are duplicates.</t>
+  </si>
+  <si>
+    <t>All files except demographics.csv should be throwing error messages for duplicates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -595,6 +643,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -673,7 +728,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -722,6 +777,19 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1098,56 +1166,56 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.1640625" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="82.125" customWidth="1"/>
+    <col min="2" max="2" width="49.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="22"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1163,30 +1231,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="35.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1212,132 +1280,132 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="170.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>160</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G8">
         <f>SUM(33-5)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1361,39 +1429,197 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="46.875" customWidth="1"/>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
+    <col min="6" max="6" width="78.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.625" style="5" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.58203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.08203125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="5"/>
+    <col min="5" max="5" width="33.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1414,391 +1640,391 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="F7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="77.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="E17" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -1812,7 +2038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
@@ -1820,29 +2046,29 @@
       <selection activeCell="C32" sqref="C32:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.4140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="14.4140625" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1868,73 +2094,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>73</v>
+      <c r="B3" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>117</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>120</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -1942,11 +2168,11 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -1954,11 +2180,11 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -1966,11 +2192,11 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -1978,11 +2204,11 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -1990,11 +2216,11 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2002,191 +2228,191 @@
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>74</v>
+      <c r="B12" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="E12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="F12" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="20"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="F13" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>117</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="F14" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" s="20"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="20"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
     </row>
-    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>17</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
     </row>
-    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>19</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -2194,53 +2420,53 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>75</v>
+      <c r="B22" s="25" t="s">
+        <v>74</v>
       </c>
       <c r="C22" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="E22" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="F22" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="20"/>
+      <c r="B23" s="25"/>
       <c r="C23" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="20"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -2248,11 +2474,11 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="20"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
@@ -2260,11 +2486,11 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -2272,11 +2498,11 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B27" s="20"/>
+      <c r="B27" s="25"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -2284,11 +2510,11 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
@@ -2296,11 +2522,11 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="20"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
@@ -2308,11 +2534,11 @@
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B30" s="20"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
@@ -2320,11 +2546,11 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="20"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
@@ -2332,33 +2558,33 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>76</v>
+      <c r="B32" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="C32" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="E32" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="F32" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>113</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="20"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
@@ -2366,11 +2592,11 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
@@ -2378,11 +2604,11 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="20"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
@@ -2390,11 +2616,11 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="20"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
@@ -2402,11 +2628,11 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
@@ -2414,11 +2640,11 @@
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="20"/>
+      <c r="B38" s="25"/>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
@@ -2426,11 +2652,11 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="20"/>
+      <c r="B39" s="25"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
@@ -2438,11 +2664,11 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="20"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
@@ -2450,11 +2676,11 @@
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="20"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
@@ -2462,11 +2688,11 @@
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -2487,7 +2713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -2495,31 +2721,31 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="48.08203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.4140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="48.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="1"/>
+    <col min="7" max="7" width="15.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2545,69 +2771,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -2619,7 +2845,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2631,7 +2857,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2643,7 +2869,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -2655,7 +2881,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -2667,7 +2893,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -2679,7 +2905,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -2699,7 +2925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -2707,28 +2933,28 @@
       <selection activeCell="F12" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="5"/>
-    <col min="2" max="2" width="58.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="5"/>
+    <col min="2" max="2" width="58.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="5" customWidth="1"/>
     <col min="6" max="6" width="20.25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.4140625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="5"/>
+    <col min="7" max="7" width="13.375" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2754,80 +2980,80 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>111</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Changed and updated test cases for Bootstrap
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="169">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -517,9 +517,6 @@
     <t>Bootstrap success. However, 6 error messages are returned to admin. Row 1 will consist of invalid location-id error. Row 5,6,20 will consist of invalid mac address error. Row 7 will consist of invalid timestamp error. Row 9 will consist of a duplicate of row 8. Rows 1,5,6,7,9,20 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
   <si>
-    <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
-  </si>
-  <si>
     <t>File: ab-test-1.zip</t>
   </si>
   <si>
@@ -563,6 +560,12 @@
   </si>
   <si>
     <t>All files except demographics.csv should be throwing error messages for duplicates</t>
+  </si>
+  <si>
+    <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
+  </si>
+  <si>
+    <t>Same as expected</t>
   </si>
 </sst>
 </file>
@@ -1231,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1299,14 +1302,19 @@
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1318,7 +1326,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>152</v>
+        <v>167</v>
+      </c>
+      <c r="G4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
@@ -1326,7 +1340,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -1339,6 +1353,12 @@
       </c>
       <c r="F5" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
@@ -1346,7 +1366,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -1359,6 +1379,12 @@
       </c>
       <c r="F6" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
@@ -1366,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -1379,6 +1405,12 @@
       </c>
       <c r="F7" s="3" t="s">
         <v>151</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
@@ -1386,7 +1418,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
@@ -1400,9 +1432,11 @@
       <c r="F8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G8">
-        <f>SUM(33-5)</f>
-        <v>28</v>
+      <c r="G8" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1477,19 +1511,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="20"/>
@@ -1499,19 +1533,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
@@ -1521,19 +1555,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>155</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
@@ -1543,19 +1577,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -1565,19 +1599,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test results for login function
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="60" windowWidth="19430" windowHeight="12170" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="169">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -517,6 +517,9 @@
     <t>Bootstrap success. However, 6 error messages are returned to admin. Row 1 will consist of invalid location-id error. Row 5,6,20 will consist of invalid mac address error. Row 7 will consist of invalid timestamp error. Row 9 will consist of a duplicate of row 8. Rows 1,5,6,7,9,20 will not be displayed in the database. All other rows should be displayed correctly.</t>
   </si>
   <si>
+    <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 5,6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,5,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
+  </si>
+  <si>
     <t>File: ab-test-1.zip</t>
   </si>
   <si>
@@ -562,10 +565,7 @@
     <t>All files except demographics.csv should be throwing error messages for duplicates</t>
   </si>
   <si>
-    <t>Bootstrap success. However, 8 error messages are returned to admin. Row 3,4 will consist of mac-address error. Row 6,7 will consist of password error. Row 8,9 will consist of email error. Row 10 will consist of gender error. Rows 3,4,6,7,8,9,10 will not be displayed in the database. All other rows should be displayed correctly.</t>
-  </si>
-  <si>
-    <t>Same as expected</t>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -765,9 +765,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -808,6 +805,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1169,19 +1175,19 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="82.125" customWidth="1"/>
-    <col min="2" max="2" width="49.375" customWidth="1"/>
+    <col min="1" max="1" width="82.08203125" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
+      <c r="A1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="22"/>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="21"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>87</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
@@ -1197,7 +1203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>95</v>
       </c>
@@ -1205,7 +1211,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>94</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>93</v>
       </c>
@@ -1234,30 +1240,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="35.875" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1283,12 +1289,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1302,19 +1308,14 @@
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1326,21 +1327,15 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="G4" t="s">
-        <v>168</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -1354,19 +1349,13 @@
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -1380,19 +1369,13 @@
       <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -1406,19 +1389,13 @@
       <c r="F7" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
@@ -1432,14 +1409,12 @@
       <c r="F8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>SUM(33-5)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1469,149 +1444,149 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.75" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.25" customWidth="1"/>
-    <col min="6" max="6" width="78.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+    <row r="2" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F5" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>2</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>3</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>4</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1621,34 +1596,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.58203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="33.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="5"/>
+    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.58203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.58203125" style="5"/>
+    <col min="9" max="9" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.58203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="I1" s="28">
+        <v>42281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1674,7 +1654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="62" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1699,8 +1679,11 @@
       <c r="H3" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I3" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1725,8 +1708,11 @@
       <c r="H4" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I4" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1751,8 +1737,11 @@
       <c r="H5" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="I5" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1777,8 +1766,11 @@
       <c r="H6" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I6" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1800,8 +1792,11 @@
       <c r="H7" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="I7" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1826,8 +1821,11 @@
       <c r="H8" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="I8" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1852,8 +1850,11 @@
       <c r="H9" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I9" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1878,8 +1879,11 @@
       <c r="H10" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I10" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1901,8 +1905,11 @@
       <c r="H11" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I11" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1927,8 +1934,11 @@
       <c r="H12" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I12" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1953,8 +1963,11 @@
       <c r="H13" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I13" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1979,8 +1992,11 @@
       <c r="H14" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I14" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -2005,60 +2021,69 @@
       <c r="H15" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="I15" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="26" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="26">
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="I16" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="26" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="26">
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2080,29 +2105,29 @@
       <selection activeCell="C32" sqref="C32:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="7" max="7" width="13.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2128,611 +2153,611 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="24"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="B11" s="24"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
         <v>11</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
         <v>14</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="12">
         <v>15</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="15" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="12">
         <v>16</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="15" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="12">
         <v>17</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="15" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="12">
         <v>18</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
         <v>19</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+    </row>
+    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="15" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="24"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="24"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+    </row>
+    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="24"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="24"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="24"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="24"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="24"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="24"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="24"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="24"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2755,31 +2780,31 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="48.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" style="1"/>
+    <col min="2" max="2" width="48.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.08203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2805,7 +2830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2827,7 +2852,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -2849,7 +2874,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -2867,7 +2892,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -2879,7 +2904,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2891,7 +2916,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2903,7 +2928,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -2915,7 +2940,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -2927,7 +2952,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -2939,7 +2964,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -2967,28 +2992,28 @@
       <selection activeCell="F12" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="5"/>
-    <col min="2" max="2" width="58.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.58203125" style="5"/>
+    <col min="2" max="2" width="58.08203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="20.25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="5"/>
+    <col min="7" max="7" width="13.33203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.58203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3014,25 +3039,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -3052,42 +3077,42 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Fixed Bug Test update Fixed the test cases for Bootstrap and Addbatch.
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="60" windowWidth="19430" windowHeight="12170" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>Values printed as expected</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -784,12 +787,18 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -805,15 +814,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1175,19 +1175,19 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.08203125" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="82.125" customWidth="1"/>
+    <col min="2" max="2" width="49.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.6">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="21"/>
-    </row>
-    <row r="2" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>87</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>95</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>94</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>93</v>
       </c>
@@ -1240,30 +1240,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="35.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.875" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1308,9 +1308,14 @@
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="G3" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1329,8 +1334,14 @@
       <c r="F4" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+      <c r="G4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1349,8 +1360,14 @@
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="G5" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1369,8 +1386,14 @@
       <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="G6" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1389,8 +1412,14 @@
       <c r="F7" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="G7" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1409,12 +1438,14 @@
       <c r="F8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="G8">
-        <f>SUM(33-5)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G8" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1441,21 +1472,21 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.75" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="46.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="46.875" customWidth="1"/>
+    <col min="4" max="4" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="17.25" customWidth="1"/>
-    <col min="6" max="6" width="78.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="78.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1500,10 +1531,14 @@
       <c r="F2" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
@@ -1522,10 +1557,14 @@
       <c r="F3" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>3</v>
       </c>
@@ -1544,10 +1583,14 @@
       <c r="F4" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -1563,13 +1606,17 @@
       <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -1587,6 +1634,12 @@
       </c>
       <c r="F6" s="17" t="s">
         <v>165</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1598,37 +1651,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I17"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.58203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.625" style="5" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.58203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.08203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.58203125" style="5"/>
-    <col min="9" max="9" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.58203125" style="5"/>
+    <col min="5" max="5" width="33.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.625" style="5"/>
+    <col min="9" max="9" width="10.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="I1" s="28">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="I1" s="22">
         <v>42281</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1683,7 +1736,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1712,7 +1765,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1741,7 +1794,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1770,7 +1823,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1796,7 +1849,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1825,7 +1878,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1854,7 +1907,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1883,7 +1936,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1909,7 +1962,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1938,7 +1991,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1967,7 +2020,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1996,7 +2049,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -2025,65 +2078,65 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="26" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+    <row r="16" spans="1:9" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
         <v>14</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="20" t="s">
         <v>108</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="26" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="26">
+    <row r="17" spans="1:9" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
         <v>15</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="20" t="s">
         <v>108</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2105,29 +2158,29 @@
       <selection activeCell="C32" sqref="C32:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.58203125" customWidth="1"/>
+    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.08203125" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2153,11 +2206,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2175,11 +2228,11 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="14" t="s">
         <v>113</v>
       </c>
@@ -2195,11 +2248,11 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="14" t="s">
         <v>117</v>
       </c>
@@ -2215,11 +2268,11 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
@@ -2227,11 +2280,11 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2239,11 +2292,11 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
-      <c r="B8" s="24"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -2251,11 +2304,11 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="24"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -2263,11 +2316,11 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -2275,11 +2328,11 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
@@ -2287,11 +2340,11 @@
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="26" t="s">
         <v>73</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2309,11 +2362,11 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>11</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="14" t="s">
         <v>113</v>
       </c>
@@ -2329,11 +2382,11 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
     </row>
-    <row r="14" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="24"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="14" t="s">
         <v>120</v>
       </c>
@@ -2349,11 +2402,11 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>13</v>
       </c>
-      <c r="B15" s="24"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="14" t="s">
         <v>124</v>
       </c>
@@ -2367,11 +2420,11 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>14</v>
       </c>
-      <c r="B16" s="24"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="14" t="s">
         <v>125</v>
       </c>
@@ -2387,11 +2440,11 @@
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>15</v>
       </c>
-      <c r="B17" s="24"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="14" t="s">
         <v>126</v>
       </c>
@@ -2407,11 +2460,11 @@
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>16</v>
       </c>
-      <c r="B18" s="24"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="14" t="s">
         <v>127</v>
       </c>
@@ -2427,11 +2480,11 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>17</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="14" t="s">
         <v>128</v>
       </c>
@@ -2447,11 +2500,11 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>18</v>
       </c>
-      <c r="B20" s="24"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="14" t="s">
         <v>129</v>
       </c>
@@ -2467,11 +2520,11 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>19</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -2479,11 +2532,11 @@
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="26" t="s">
         <v>74</v>
       </c>
       <c r="C22" s="14" t="s">
@@ -2501,11 +2554,11 @@
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
     </row>
-    <row r="23" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="24"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="14" t="s">
         <v>143</v>
       </c>
@@ -2521,11 +2574,11 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="24"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
@@ -2533,11 +2586,11 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
-      <c r="B25" s="24"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -2545,11 +2598,11 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>24</v>
       </c>
-      <c r="B26" s="24"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -2557,11 +2610,11 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>25</v>
       </c>
-      <c r="B27" s="24"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -2569,11 +2622,11 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>26</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -2581,11 +2634,11 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
-      <c r="B29" s="24"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
@@ -2593,11 +2646,11 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
@@ -2605,11 +2658,11 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="24"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -2617,11 +2670,11 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C32" s="14" t="s">
@@ -2639,11 +2692,11 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
@@ -2651,11 +2704,11 @@
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -2663,11 +2716,11 @@
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="24"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
@@ -2675,11 +2728,11 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
@@ -2687,11 +2740,11 @@
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -2699,11 +2752,11 @@
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="24"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
@@ -2711,11 +2764,11 @@
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="24"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
@@ -2723,11 +2776,11 @@
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="24"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -2735,11 +2788,11 @@
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="24"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
@@ -2747,11 +2800,11 @@
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
@@ -2780,31 +2833,31 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="1"/>
-    <col min="2" max="2" width="48.08203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="1"/>
+    <col min="2" max="2" width="48.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.58203125" style="1"/>
+    <col min="7" max="7" width="15.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2830,7 +2883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -2852,7 +2905,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -2874,7 +2927,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -2892,7 +2945,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -2904,7 +2957,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2916,7 +2969,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2928,7 +2981,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -2940,7 +2993,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -2952,7 +3005,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -2964,7 +3017,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -2992,28 +3045,28 @@
       <selection activeCell="F12" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.58203125" style="5"/>
-    <col min="2" max="2" width="58.08203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.08203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="5"/>
+    <col min="2" max="2" width="58.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="5" customWidth="1"/>
     <col min="6" max="6" width="20.25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.58203125" style="5"/>
+    <col min="7" max="7" width="13.375" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3039,7 +3092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -3057,7 +3110,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="93" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -3077,42 +3130,42 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added overuse test cases, added basic app test (which is done already)
</commit_message>
<xml_diff>
--- a/testing/TESTCASE.xlsx
+++ b/testing/TESTCASE.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhihui/NetBeansProjects/is203_g3t3/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="60" windowWidth="19425" windowHeight="12165" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="DeleteLocation" sheetId="4" r:id="rId6"/>
     <sheet name="SmartPhoneUsageHeatmap" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="167">
   <si>
     <t>TEST CASES</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Enter valid emailID and valid password but the password in Capital Letters</t>
   </si>
   <si>
-    <t>Usage time category</t>
-  </si>
-  <si>
     <t>Usage time category and demographics</t>
   </si>
   <si>
@@ -403,102 +400,18 @@
     <t>invalid timestamp</t>
   </si>
   <si>
-    <t>invalid timestamp format</t>
-  </si>
-  <si>
-    <t>enter wrong format of timing</t>
-  </si>
-  <si>
     <t>error msg: please fill in correct timestamp</t>
   </si>
   <si>
-    <t>valid start date and end date</t>
-  </si>
-  <si>
     <t>start time and end time</t>
   </si>
   <si>
-    <t>enter a start time and end time</t>
-  </si>
-  <si>
     <t>valid start and end time plus checked year,checked gender and checked school option</t>
   </si>
   <si>
-    <t>start date and end date with all three additional check box info checked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enter start time and end time and tick all the boxes. </t>
-  </si>
-  <si>
-    <t>3  tables for each usage level with the count of users in the category</t>
-  </si>
-  <si>
-    <t>valid start and end time plus checked year option</t>
-  </si>
-  <si>
     <t>valid start and end time plus checked gender option</t>
   </si>
   <si>
-    <t>valid start and end time plus checked school option</t>
-  </si>
-  <si>
-    <t>valid start and end time plus checked year and checked gender option</t>
-  </si>
-  <si>
-    <t>valid start and end time plus checked year and checked school option</t>
-  </si>
-  <si>
-    <t>valid start and end time plus checked gender and checked school option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time plus checked year option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time plus checked gender option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time plus checked school option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time  plus checked year and checked gender option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time plus checked year and checked school option</t>
-  </si>
-  <si>
-    <t>enter a start time and end time  plus checked gender and checked school option</t>
-  </si>
-  <si>
-    <t>3  tables for each usage level. Users break down and categorised by gender then year and then school</t>
-  </si>
-  <si>
-    <t>3  tables for each usage level. Users break down and categorised by gender then school</t>
-  </si>
-  <si>
-    <t>3  tables for each usage level. Users break down and categorised by  year and then school</t>
-  </si>
-  <si>
-    <t>3  tables for each usage level. Users break down and categorised by gender then year</t>
-  </si>
-  <si>
-    <t>3  tables for each usage level. Users break down and categorised  school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3  tables for each usage level. Users break down and categorised by gender </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3  tables for each usage level. Users break down and categorised by year </t>
-  </si>
-  <si>
-    <t xml:space="preserve">valid start and end time </t>
-  </si>
-  <si>
-    <t>1 table and categorized by app name and each app shows the daily usage hours and percentage</t>
-  </si>
-  <si>
-    <t>start date and end date</t>
-  </si>
-  <si>
     <t>valid start and end time</t>
   </si>
   <si>
@@ -569,13 +482,261 @@
   </si>
   <si>
     <t>Values printed as expected</t>
+  </si>
+  <si>
+    <t>correct result shown</t>
+  </si>
+  <si>
+    <t>start date : 06/04/2015
+end date: 06/04/2015</t>
+  </si>
+  <si>
+    <t>Intense Users count: 0 
+Intense Percent: 0%
+Normal Users count: 7
+Normal Percent: 7%
+Mild Users count: 100
+Mild Percent: 93%</t>
+  </si>
+  <si>
+    <t>Usage time category
+(data v1)</t>
+  </si>
+  <si>
+    <t>Please fill out this fields</t>
+  </si>
+  <si>
+    <t>Intense Users count: 0 
+Intense Percent: 0%
+Normal Users count: 0
+Normal Percent: 0%
+Mild Users count: 0
+Mild Percent: 0%</t>
+  </si>
+  <si>
+    <t>start date : 06/04/0000
+end date: 06/04/0000</t>
+  </si>
+  <si>
+    <t>start date : 06/04/2015
+end date: 06/04/2015
+Filter: gender, school, year</t>
+  </si>
+  <si>
+    <t>start date : 06/04/0001
+end date: 06/04/0001
+Filter: gender, school, year</t>
+  </si>
+  <si>
+    <t>1. At top navbar, click Basic App Usage dropdown and select 'Basic App (with demographic)
+2. put in all the input according to input column and click submit</t>
+  </si>
+  <si>
+    <t>1. At top navbar, click Basic App Usage dropdown and select 'Basic App (with demographic)
+2. click submit</t>
+  </si>
+  <si>
+    <t>start date : 06/04/2015
+end date: 06/04/2015
+Filter: gender, school</t>
+  </si>
+  <si>
+    <t>valid start and end time plus select gender, school option</t>
+  </si>
+  <si>
+    <t>3  tables for each usage level. Users break down and categorised by gender then school and then year
+M,55,51%
+- business, 10, 18%
+--- 2011,1,10%
+-----intense,0,0%
+-----normal,0,0%
+-----mild,1,100%
+--- 2012,3,30%
+-----intense,0,0%
+-----normal,1,33%
+-----mild,2,67%
+--- 2013,0,0%
+--- 2014,2,20%
+--- 2015,4,40%
+- accountancy,3,5%
+--- 2011,0,0%
+--- 2012,1,33%
+--- 2013,2,67%
+--- 2014,0,0%
+--- 2015,0,0%
+F, 52, 49%
+- business,6,12%
+---2011,1,17%
+-----intense,0,0%
+-----normal,0,0%
+-----mild,1,100%
+---2012,2,33%
+-----intense,0,0%
+-----normal,1,50%
+-----mild,1,50%
+---2013,0,0%
+---2014,0,0%
+---2015,3,50%
+- accountancy, 10, 19%
+---2011,2,20%
+---2012,1,10%
+---2013,1,10%
+---2014,4,40%
+---2015,2,20%</t>
+  </si>
+  <si>
+    <t>2  tables for each usage level. Users break down and categorised by gender then school
+M,55,51%
+- business, 10, 18%
+---intense,0,0%
+---normal,1,10%
+---mild,9,90%
+- accountancy,3,5%
+---intense,0,0%
+---normal,0,0%
+---mild,3,100%
+F, 52, 49%
+- business,6,12%
+---intense,0,0%
+---normal,1,17%
+---mild,5,83%
+- accountancy, 10, 19%
+---intense,0,0%
+---normal,0,0%
+---mild,10,100%</t>
+  </si>
+  <si>
+    <t>valid start and end time plus checked gender</t>
+  </si>
+  <si>
+    <t>1 tables for each usage level. Users break down and categorised by gender then school
+M,55,51%
+---intense,0,0%
+---normal,6,11%
+---mild,49,89%
+F, 52, 49%
+---intense,0,0%
+---normal,1,2%
+---mild,51,98%</t>
+  </si>
+  <si>
+    <t>1. At top navbar, click Basic App Usage dropdown and select 'App Category'
+2. put in all the input according to input column and click submit</t>
+  </si>
+  <si>
+    <t>Invalid Date. Please select your desired date again</t>
+  </si>
+  <si>
+    <t>Books,3437,2%
+Education,527,0%
+Entertainment,3701,2%
+Fitness,0,0%
+Games,2674,2%
+Information,2861,2%
+Library,0,0%
+Local,1206,1%
+Others,70712,46%
+Social,67113,43%
+Tools,2530,2%</t>
+  </si>
+  <si>
+    <t>00.00-01.00,0
+01.00-02.00,0
+02.00-03.00,0
+03.00-04.00,0
+04.00-05.00,0
+05.00-06.00,0
+06.00-07.00,0
+07.00-08.00,0
+08.00-09.00,0
+09.00-10.00,0
+10.00-11.00,0
+11.00-12.00,0
+12.00-13.00,0
+13.00-14.00,0
+14.00-15.00,0
+15.00-16.00,0
+16.00-17.00,0
+17.00-18.00,0
+18.00-19.00,0
+19.00-20.00,0
+20.00-21.00,0
+21.00-22.00,0
+22.00-23.00,0
+23.00-00.00,0</t>
+  </si>
+  <si>
+    <t>1. At top navbar, click Basic App Usage dropdown and select 'Diurnal Report'
+2. put in all the input according to input column and click submit</t>
+  </si>
+  <si>
+    <t>start date : 06/04/2015
+end date: 06/04/2015
+Filter: gender=NA, school=NA, year=NA</t>
+  </si>
+  <si>
+    <t>00.00-01.00,0
+01.00-02.00,0
+02.00-03.00,0
+03.00-04.00,0
+04.00-05.00,0
+05.00-06.00,0
+06.00-07.00,0
+07.00-08.00,0
+08.00-09.00,0
+09.00-10.00,0
+10.00-11.00,0
+11.00-12.00,0
+12.00-13.00,0
+13.00-14.00,523
+14.00-15.00,506
+15.00-16.00,408
+16.00-17.00,0
+17.00-18.00,0
+18.00-19.00,0
+19.00-20.00,0
+20.00-21.00,0
+21.00-22.00,0
+22.00-23.00,0
+23.00-00.00,0</t>
+  </si>
+  <si>
+    <t>start date : 06/04/2015
+end date: 06/04/2015
+Filter: gender=M, school=economics, year=NA</t>
+  </si>
+  <si>
+    <t>00.00-01.00,0
+01.00-02.00,0
+02.00-03.00,0
+03.00-04.00,0
+04.00-05.00,0
+05.00-06.00,0
+06.00-07.00,0
+07.00-08.00,0
+08.00-09.00,0
+09.00-10.00,0
+10.00-11.00,0
+11.00-12.00,0
+12.00-13.00,0
+13.00-14.00,345
+14.00-15.00,512
+15.00-16.00,383
+16.00-17.00,0
+17.00-18.00,0
+18.00-19.00,0
+19.00-20.00,0
+20.00-21.00,0
+21.00-22.00,0
+22.00-23.00,0
+23.00-00.00,0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -660,6 +821,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -734,7 +903,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -814,6 +983,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1175,56 +1347,56 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="82.125" customWidth="1"/>
-    <col min="2" max="2" width="49.375" customWidth="1"/>
+    <col min="1" max="1" width="82.1640625" customWidth="1"/>
+    <col min="2" max="2" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="B2" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1240,21 +1412,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="66" zoomScalePageLayoutView="66" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="35.875" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1435,7 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1289,12 +1461,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1309,18 +1481,18 @@
         <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="141.75" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
@@ -1332,21 +1504,21 @@
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -1361,18 +1533,18 @@
         <v>16</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -1387,18 +1559,18 @@
         <v>24</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="157.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>21</v>
@@ -1410,21 +1582,21 @@
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>22</v>
@@ -1436,16 +1608,16 @@
         <v>11</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1459,11 +1631,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1475,18 +1642,18 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="46.875" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="17.25" customWidth="1"/>
-    <col min="6" max="6" width="78.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="78.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
@@ -1512,56 +1679,56 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,77 +1736,77 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1651,25 +1818,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="40.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="33.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="5"/>
-    <col min="9" max="9" width="10.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.625" style="5"/>
+    <col min="5" max="5" width="33.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="5"/>
+    <col min="9" max="9" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1848,7 @@
         <v>42281</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1707,7 +1874,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1727,16 +1894,16 @@
         <v>32</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1756,16 +1923,16 @@
         <v>37</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1785,16 +1952,16 @@
         <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1814,16 +1981,16 @@
         <v>37</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1837,19 +2004,19 @@
         <v>45</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1866,19 +2033,19 @@
         <v>48</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1895,19 +2062,19 @@
         <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1924,19 +2091,19 @@
         <v>33</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1950,19 +2117,19 @@
         <v>53</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1979,19 +2146,19 @@
         <v>56</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -2008,19 +2175,19 @@
         <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -2040,16 +2207,16 @@
         <v>37</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -2069,16 +2236,16 @@
         <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="20" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -2098,16 +2265,16 @@
         <v>37</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="20" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="20" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -2127,16 +2294,16 @@
         <v>37</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2152,23 +2319,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
-    <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2347,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2206,72 +2373,78 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>111</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>2</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
       <c r="B4" s="26"/>
       <c r="C4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>3</v>
-      </c>
+      <c r="G4" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
       <c r="B5" s="26"/>
       <c r="C5" s="14" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
-        <v>4</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
       <c r="B6" s="26"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -2280,10 +2453,8 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>5</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
       <c r="B7" s="26"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2292,10 +2463,8 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>6</v>
-      </c>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
       <c r="B8" s="26"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -2304,10 +2473,8 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>7</v>
-      </c>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
       <c r="B9" s="26"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -2316,10 +2483,8 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>8</v>
-      </c>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
       <c r="B10" s="26"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -2328,255 +2493,265 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>73</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B12" s="26"/>
       <c r="C12" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="409" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="330" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="14" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="14"/>
+        <v>156</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="E15" s="14" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="26"/>
-      <c r="C16" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>141</v>
-      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
     </row>
-    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="26"/>
-      <c r="C17" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>140</v>
-      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="26"/>
-      <c r="C18" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>139</v>
-      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="26"/>
-      <c r="C19" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>138</v>
-      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="26"/>
-      <c r="C20" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>137</v>
-      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>19</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="135" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>20</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>74</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B22" s="26"/>
       <c r="C22" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-    </row>
-    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="165" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="14"/>
@@ -2586,9 +2761,9 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="14"/>
@@ -2598,9 +2773,9 @@
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="14"/>
@@ -2610,9 +2785,9 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="14"/>
@@ -2622,9 +2797,9 @@
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="14"/>
@@ -2634,9 +2809,9 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="14"/>
@@ -2646,9 +2821,9 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="14"/>
@@ -2658,67 +2833,107 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
-        <v>29</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="360" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
-        <v>30</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>75</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B32" s="26"/>
       <c r="C32" s="14" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="360" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="360" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="26"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="13"/>
@@ -2728,9 +2943,9 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="13"/>
@@ -2740,9 +2955,9 @@
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="13"/>
@@ -2752,9 +2967,9 @@
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="13"/>
@@ -2764,9 +2979,9 @@
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="13"/>
@@ -2776,9 +2991,9 @@
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="13"/>
@@ -2788,9 +3003,9 @@
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="13"/>
@@ -2800,25 +3015,13 @@
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>40</v>
-      </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="B12:B21"/>
-    <mergeCell ref="B22:B31"/>
-    <mergeCell ref="B32:B42"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="B31:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2833,19 +3036,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="48.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="48.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="1"/>
+    <col min="7" max="7" width="15.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -2857,7 +3060,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2883,69 +3086,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="D5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -2957,7 +3160,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -2969,7 +3172,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -2981,7 +3184,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -2993,7 +3196,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -3005,7 +3208,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -3017,7 +3220,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -3045,19 +3248,19 @@
       <selection activeCell="F12" sqref="F10:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="5"/>
-    <col min="2" max="2" width="58.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.625" style="5"/>
+    <col min="1" max="1" width="8.6640625" style="5"/>
+    <col min="2" max="2" width="58.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -3066,7 +3269,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3092,80 +3295,80 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>111</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>

</xml_diff>